<commit_message>
sanofi migration step 28
</commit_message>
<xml_diff>
--- a/Projects/SANOFICN/Data/Test_Template.xlsx
+++ b/Projects/SANOFICN/Data/Test_Template.xlsx
@@ -24,6 +24,8 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'Route Plan Compliance'!$A$1:$E$768</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Route Plan Compliance'!$A$1:$E$768</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Route Plan Compliance'!$A$1:$E$768</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Route Plan Compliance'!$A$1:$E$768</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Route Plan Compliance'!$A$1:$E$768</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -850,7 +852,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="57">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -928,6 +930,9 @@
   </si>
   <si>
     <t xml:space="preserve">Survey Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SURVEY_QUESTION</t>
   </si>
   <si>
     <t xml:space="preserve">Perfect Store</t>
@@ -1793,18 +1798,18 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1781376518219"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.2226720647773"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.0121457489879"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1984,7 +1989,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1998,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>9</v>
@@ -2014,10 +2019,10 @@
     </row>
     <row r="11" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="7" t="s">
@@ -2029,10 +2034,10 @@
     </row>
     <row r="12" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="8" t="s">
@@ -2044,10 +2049,10 @@
     </row>
     <row r="13" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="10" t="s">
@@ -2059,14 +2064,14 @@
     </row>
     <row r="14" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="16"/>
@@ -2098,12 +2103,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="43.4898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="18" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="18" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="18" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="19" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="8.89068825910931"/>
@@ -2118,7 +2123,7 @@
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2126,25 +2131,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,16 +2161,16 @@
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="29" t="n">
         <v>1</v>
@@ -2196,13 +2201,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="30" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="30" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="30" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="30" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="30" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="30" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2215,7 +2220,7 @@
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
       <c r="H1" s="32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2223,25 +2228,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>36</v>
-      </c>
       <c r="H2" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,13 +2409,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="38" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="38" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="38" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="38" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="39" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="38" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="38" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="38" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="38" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="39" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="40" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2423,7 +2428,7 @@
       <c r="F1" s="41"/>
       <c r="G1" s="41"/>
       <c r="H1" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2431,25 +2436,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>36</v>
-      </c>
       <c r="H2" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2477,13 +2482,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="30" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="45" width="8.89068825910931"/>
   </cols>
@@ -2497,7 +2502,7 @@
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" s="46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2505,25 +2510,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2551,12 +2556,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="43.4898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="48" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="49" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="50" width="8.89068825910931"/>
@@ -2571,7 +2576,7 @@
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
       <c r="H1" s="46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
@@ -3595,25 +3600,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
@@ -4641,16 +4646,16 @@
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="53" t="n">
         <v>6955206300031</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="56" t="n">
         <v>2</v>
@@ -4665,16 +4670,16 @@
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="53" t="n">
         <v>6955206300031</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H4" s="56" t="n">
         <v>1</v>
@@ -4705,11 +4710,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="37.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="37.8137651821862"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="59" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4718,28 +4723,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="26" t="n">
         <v>43466</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="59" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" s="59" t="n">
         <v>2</v>
@@ -4772,10 +4777,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="60" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="60" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="60" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="60" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="60" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="60" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="11" min="7" style="60" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
@@ -4799,19 +4804,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="61" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
@@ -4821,16 +4826,16 @@
     </row>
     <row r="3" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="60" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="63" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="60" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G3" s="64"/>
       <c r="H3" s="64"/>
@@ -4840,16 +4845,16 @@
     </row>
     <row r="4" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="60" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="64"/>
       <c r="H4" s="64"/>
@@ -4859,16 +4864,16 @@
     </row>
     <row r="5" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="60" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="65" t="s">
-        <v>54</v>
-      </c>
       <c r="F5" s="64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>

</xml_diff>